<commit_message>
Updated ISL model - 2025-08-01 00:24
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E193A012-58FB-44EB-8229-C1D5B1157B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5DC9EDE-4D98-4731-9AA5-4530629FD30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{DACF5E50-8F44-462E-9229-D081CCFA02F7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{D7FC5DB6-F9B7-46AE-935E-4B38129B13B3}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0281BF5-AD85-477B-A179-BF415B6B668A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E502DF3-2BD7-48A1-8241-79FDD2F33C31}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F52D1B4-D75E-4C9F-9727-E5F8E062BD33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BED4BE7-5D52-4C09-9DAF-A4CA8D4BA23B}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FED9D0-31CF-4D8F-AA85-82708640570D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28A0D45-E73F-4D65-9BBC-4DC8EA7F6FD1}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 00:35
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78E6BD3F-43A3-4D34-953B-141242301330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B26A4A1-F357-48CA-BDD8-240745100EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{CFAC185F-60F0-482B-81B3-C13586396144}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{5E44BC7D-71E1-4726-B85D-E849491D41BB}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE6AE0D0-334B-4DFB-8C38-F9F027A401D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF0655E-D96E-49BA-9C36-A481D298912B}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3CAE1C-2332-4EE6-9753-AC6338D2B864}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3066B4-D90D-4CA4-A74E-75E506C843F1}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD08BD33-FA8D-41E0-BAB9-A498AD05E569}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C522F4A8-8447-47F4-B9F6-7D0A00A2EE5A}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 00:47
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B26A4A1-F357-48CA-BDD8-240745100EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2F442C8-4D34-48B5-89DC-69D5E94F5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{5E44BC7D-71E1-4726-B85D-E849491D41BB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{5CD362B9-EB53-4189-80B6-021B41D83C51}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF0655E-D96E-49BA-9C36-A481D298912B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC589235-9A74-4401-B35C-14608131F14E}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3066B4-D90D-4CA4-A74E-75E506C843F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0B9932-8F52-4E88-95F6-70803AA5BFE7}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C522F4A8-8447-47F4-B9F6-7D0A00A2EE5A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D422C28-BB2C-4338-A659-C90DD8F67BD2}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 00:49
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2F442C8-4D34-48B5-89DC-69D5E94F5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FCC92B6-CE03-456C-8F3C-388929B5312D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{5CD362B9-EB53-4189-80B6-021B41D83C51}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{D7DE1E53-74B2-4629-984B-21BEBDED882A}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC589235-9A74-4401-B35C-14608131F14E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B4D7C8-90BE-4196-BA53-59729568FB3C}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0B9932-8F52-4E88-95F6-70803AA5BFE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09380FA5-C5F7-464A-8BCF-D3E73D5F4203}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D422C28-BB2C-4338-A659-C90DD8F67BD2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E271859-FCA7-4A54-83FA-790C78C61DE2}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 00:59
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FCC92B6-CE03-456C-8F3C-388929B5312D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEBB22AC-7B2C-4603-9B95-1A41CD8AEB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{D7DE1E53-74B2-4629-984B-21BEBDED882A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{C1D5DAAB-E7E1-486E-960D-102F1BBCC64C}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B4D7C8-90BE-4196-BA53-59729568FB3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97061EAF-98F1-4CF2-8E49-4A6B9A03E07E}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09380FA5-C5F7-464A-8BCF-D3E73D5F4203}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BD944A-AF88-4CAC-BBC1-61AC686353B9}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E271859-FCA7-4A54-83FA-790C78C61DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3486D4-2E26-4EB4-9A8F-5B17F5879347}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 01:01
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEBB22AC-7B2C-4603-9B95-1A41CD8AEB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B84EF738-D95F-4184-9570-928379B08486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{C1D5DAAB-E7E1-486E-960D-102F1BBCC64C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{DB802D25-34BD-4AF3-B0F1-27FC12F048AC}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97061EAF-98F1-4CF2-8E49-4A6B9A03E07E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45674C10-838F-4601-ADE5-1C1BD1089BDF}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BD944A-AF88-4CAC-BBC1-61AC686353B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01A2A1D-0720-4124-A26D-3E0ACA578BE6}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3486D4-2E26-4EB4-9A8F-5B17F5879347}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C07E909-39CD-4129-8371-655C78B26187}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 01:02
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B84EF738-D95F-4184-9570-928379B08486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56CDC945-DCE5-4A46-A9D8-368AFF90ED3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{DB802D25-34BD-4AF3-B0F1-27FC12F048AC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{09506EAC-9D7B-4B3C-9341-4E2D03CE64DD}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45674C10-838F-4601-ADE5-1C1BD1089BDF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176E59D4-9BA4-4CF7-AFCF-ABF1C4F0740E}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01A2A1D-0720-4124-A26D-3E0ACA578BE6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A908A1-0941-40E0-93E7-51836E1E02D7}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C07E909-39CD-4129-8371-655C78B26187}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCAA209-2524-44B3-AD6B-F5CDFE1B326C}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 01:04
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56CDC945-DCE5-4A46-A9D8-368AFF90ED3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8916ECB9-A087-4ADB-B5CD-FBDC8728FDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{09506EAC-9D7B-4B3C-9341-4E2D03CE64DD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{45D257B8-40E2-4097-BF34-6B7D0ED8B8F1}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176E59D4-9BA4-4CF7-AFCF-ABF1C4F0740E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72861A0-1E62-4186-BCE4-80383B7125B7}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A908A1-0941-40E0-93E7-51836E1E02D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FCBFB9-4275-4CD7-A5DB-D242A68907A5}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCAA209-2524-44B3-AD6B-F5CDFE1B326C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752F4B97-B068-40ED-97E7-28B785696F14}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 01:07
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
+++ b/VerveStacks_ISL/vt_vervestacks_ISL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61C3CF65-D726-4A07-A017-93CE4C2DBB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60CD7BC0-5884-45B4-BDA6-77B7350A98B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{B1DFA350-C798-4F53-B906-14A5F0449EBD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{1A306834-CD47-4CAC-A5FA-A99A21207FCA}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -711,7 +711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82191681-0EE1-4FE3-B527-95CA2A2F753F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A168DC-476E-4051-B33B-D3BEC282CD69}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3636,7 +3636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEE845B-66A5-4808-AD48-5A1CAC9B0D84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EB6D88-0763-48CE-A2DB-91E83FA29896}">
   <dimension ref="A2:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3713,7 +3713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BB0DEE-4895-4124-ABC5-025D57F7B7A0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2B6053-7FBB-4051-9919-0F2C8E39FB2B}">
   <dimension ref="A2:S38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>